<commit_message>
Fixed firefox header lock and bounce problem
</commit_message>
<xml_diff>
--- a/public/data/class_action_ratings.xlsx
+++ b/public/data/class_action_ratings.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="21520" windowHeight="15340" tabRatio="500"/>
+    <workbookView xWindow="1920" yWindow="920" windowWidth="26640" windowHeight="15980" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,616 +19,685 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="165">
+  <si>
+    <t>Affirmative SF clinic</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ainsworth/Gerken</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>American Foreign Policy Issues</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gewirtz</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Antitrust</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Priest</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Antitrust</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Klevorick</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Banking Law and Regulation</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Macey</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bankruptcy</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Contemporary Issues in Law &amp; Business</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Romano</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Democracy and Distribution</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Graetz</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Democratic Constitutionalism</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Post / Siegel</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Disability Rights and Policy</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Jolls</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Environmental Law and Policy</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Elliott</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Law and Globalization</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Stone Sweet</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Treaties and International Agreements</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Brilmayer / Reisman</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Criminal Law and Administration</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Whitman</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Green Energy Policy</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Elliott</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Guantanamo</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fidell, Greeehouse</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>History of Common Law</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Langbein</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Information Privacy Law</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Jolls</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Information Society</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Balkin</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Intellectual Property</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Schwartz</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Behavioral and Institutional Economics</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shiller</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Business Organizations</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Macey</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Brooks</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Romano</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Capital Punishment</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bright</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Capitalism film society</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Challenges of General Counsel</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Solender</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Chinese Legal Reform Workshop</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gewirtz</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Con Law</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rubenfeld</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Constitutional Litigation Seminar </t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Calabresi / Walker</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Constitutional Philosophy History</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ackerman</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cont legal issues in Africa</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Brilmayer</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Contracts</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Carter</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Corruption, Economic Development, and Democracy</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rose-Ackerman</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Crim Procedure</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Duke</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Crim. Law and Admin.</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Stith</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Criminal Law and Administration</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Meares</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rubenfeld</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Class</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Teacher</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Instructor quality</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Classtime value</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Workload</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>% recommended</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>% said best teacher</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Risk factor (percentage who rate teacher 1 or 2</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Notes</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Administrative Law</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mashaw</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Teacher ratings</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Administrative Law </t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Parrillo</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Admiralty Law</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fidell</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Adv. Civil Liberties and National Security</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wishnie, Metcalf</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Advanced Legal Research</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Harrison/Kaffman/Tubs/Nann</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Advanced Legal Writing</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Harrison</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
   <si>
     <t>Regulation and Institutional Design</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Mashaw</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Torts</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Guido</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Transnational Law</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Hathaway</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>87%</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>70%</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>0%</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Trial Practice</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Pottenger/Wizner</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>US International Taxation</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Samuels</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Ayres</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>International Business Transactions</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Chua</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>International Commercial Arbitration</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Reisman</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Internet Privacy</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Cohen</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Introduction to the Philosophy of Law</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Shapiro</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Justice</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Ackerman</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Law and Prosperity</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Law of Climate Change</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Kysar</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Law of Democracy</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Gerken</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Legislation</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Eskridge</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Media Law</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Military Justice</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Fidell</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Procedure</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Resnik</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Property</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Priest</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Property</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Ellickson</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Property, Social Justice, Environment</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Rose</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Public Order of the World Community</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Reisman</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Quantitative Corporate Finance</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Ayres</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Rationality and Choice</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Jolls</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Democratic Constitutionalism</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Siegel/Post</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Efficient Techniques of Legal Research</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Kaufmann/Tubbs</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Employment Discrimination</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Jolls</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Env Protec. Clinic</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Kennedy, Esty</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Environmental Law and Policy</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Esty</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Evidence</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Duke</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Evidence</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Kahan</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Federal Courts</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Resnik</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Federal Income Taxation</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Listokin</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Markovits</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Alstott</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>First Amendment</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Balkin</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Frontiers in Organization Law</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Hansmann</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Green Energy Policy</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Elliott</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Guantanamo</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Fidell, Greeehouse</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>History of Common Law</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Langbein</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Information Privacy Law</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Jolls</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Information Society</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Balkin</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Intellectual Property</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Schwartz</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Behavioral and Institutional Economics</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Shiller</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Business Organizations</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Macey</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Brooks</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Romano</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Capital Punishment</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Bright</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Capitalism film society</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Challenges of General Counsel</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Solender</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Chinese Legal Reform Workshop</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gewirtz</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Con Law</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Rubenfeld</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Constitutional Litigation Seminar </t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Calabresi / Walker</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Constitutional Philosophy History</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Ackerman</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Cont legal issues in Africa</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Brilmayer</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Contracts</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Carter</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Corruption, Economic Development, and Democracy</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Rose-Ackerman</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Crim Procedure</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Duke</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Crim. Law and Admin.</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Stith</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Criminal Law and Administration</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Meares</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Rubenfeld</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Class</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Teacher</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Instructor quality</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Classtime value</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Workload</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>% recommended</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>% said best teacher</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Risk factor (percentage who rate teacher 1 or 2</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Notes</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Administrative Law</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Mashaw</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Teacher ratings</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Administrative Law </t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Parrillo</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Admiralty Law</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Fidell</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Adv. Civil Liberties and National Security</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Wishnie, Metcalf</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Advanced Legal Research</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Harrison/Kaffman/Tubs/Nann</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Advanced Legal Writing</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Harrison</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Affirmative SF clinic</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Ainsworth/Gerken</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>American Foreign Policy Issues</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gewirtz</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Antitrust</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Priest</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Antitrust</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Klevorick</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Banking Law and Regulation</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Macey</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Bankruptcy</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
+    <font>
+      <sz val="10"/>
+      <name val="Verdana"/>
+    </font>
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -691,31 +760,33 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -743,7 +814,7 @@
             <c:numRef>
               <c:f>Sheet1!$C$2:$C$41</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="40"/>
                 <c:pt idx="0">
                   <c:v>8.25</c:v>
@@ -769,7 +840,7 @@
                 <c:pt idx="7">
                   <c:v>9.5</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="8" formatCode="General">
                   <c:v>7.1</c:v>
                 </c:pt>
                 <c:pt idx="9">
@@ -823,7 +894,7 @@
                 <c:pt idx="25">
                   <c:v>7.1</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="26" formatCode="General">
                   <c:v>7.5</c:v>
                 </c:pt>
                 <c:pt idx="27">
@@ -869,24 +940,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="457530456"/>
-        <c:axId val="530134120"/>
+        <c:axId val="538067992"/>
+        <c:axId val="537950008"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="457530456"/>
+        <c:axId val="538067992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="530134120"/>
+        <c:crossAx val="537950008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="530134120"/>
+        <c:axId val="537950008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -894,7 +965,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="457530456"/>
+        <c:crossAx val="538067992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1268,10 +1339,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:P73"/>
+  <dimension ref="A1:P81"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="A74" sqref="A74:E81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -1289,39 +1360,39 @@
   <sheetData>
     <row r="1" spans="1:16" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
-        <v>116</v>
+        <v>71</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>117</v>
+        <v>72</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>118</v>
+        <v>73</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>119</v>
+        <v>74</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>120</v>
+        <v>75</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>121</v>
+        <v>76</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>122</v>
+        <v>77</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>123</v>
+        <v>78</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>124</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:16" s="5" customFormat="1">
       <c r="A2" s="2" t="s">
-        <v>125</v>
+        <v>80</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>126</v>
+        <v>81</v>
       </c>
       <c r="C2" s="3">
         <v>8.25</v>
@@ -1343,15 +1414,15 @@
       </c>
       <c r="I2" s="2"/>
       <c r="J2" s="5" t="s">
-        <v>127</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:16" s="5" customFormat="1">
       <c r="A3" s="2" t="s">
-        <v>128</v>
+        <v>83</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>129</v>
+        <v>84</v>
       </c>
       <c r="C3" s="3">
         <v>9.5</v>
@@ -1375,10 +1446,10 @@
     </row>
     <row r="4" spans="1:16" s="5" customFormat="1">
       <c r="A4" s="6" t="s">
-        <v>130</v>
+        <v>85</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>131</v>
+        <v>86</v>
       </c>
       <c r="C4" s="7">
         <v>8.9</v>
@@ -1403,10 +1474,10 @@
     </row>
     <row r="5" spans="1:16" s="5" customFormat="1">
       <c r="A5" s="6" t="s">
-        <v>132</v>
+        <v>87</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>133</v>
+        <v>88</v>
       </c>
       <c r="C5" s="7">
         <v>9.5</v>
@@ -1430,10 +1501,10 @@
     </row>
     <row r="6" spans="1:16" s="5" customFormat="1">
       <c r="A6" s="6" t="s">
-        <v>134</v>
+        <v>89</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>135</v>
+        <v>90</v>
       </c>
       <c r="C6" s="7">
         <v>8.3000000000000007</v>
@@ -1456,10 +1527,10 @@
     </row>
     <row r="7" spans="1:16" s="5" customFormat="1">
       <c r="A7" s="6" t="s">
-        <v>136</v>
+        <v>91</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>137</v>
+        <v>92</v>
       </c>
       <c r="C7" s="7">
         <v>8.6</v>
@@ -1482,10 +1553,10 @@
     </row>
     <row r="8" spans="1:16" s="5" customFormat="1">
       <c r="A8" s="6" t="s">
-        <v>138</v>
+        <v>0</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>139</v>
+        <v>1</v>
       </c>
       <c r="C8" s="7">
         <v>7.8750000000000009</v>
@@ -1509,10 +1580,10 @@
     </row>
     <row r="9" spans="1:16" s="11" customFormat="1">
       <c r="A9" s="2" t="s">
-        <v>140</v>
+        <v>2</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>141</v>
+        <v>3</v>
       </c>
       <c r="C9" s="3">
         <v>9.5</v>
@@ -1536,10 +1607,10 @@
     </row>
     <row r="10" spans="1:16" s="5" customFormat="1">
       <c r="A10" s="5" t="s">
-        <v>142</v>
+        <v>4</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>143</v>
+        <v>5</v>
       </c>
       <c r="C10" s="5">
         <v>7.1</v>
@@ -1563,10 +1634,10 @@
     </row>
     <row r="11" spans="1:16" s="5" customFormat="1">
       <c r="A11" s="2" t="s">
-        <v>144</v>
+        <v>6</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>145</v>
+        <v>7</v>
       </c>
       <c r="C11" s="3">
         <v>9.1999999999999993</v>
@@ -1590,10 +1661,10 @@
     </row>
     <row r="12" spans="1:16" s="10" customFormat="1">
       <c r="A12" s="5" t="s">
-        <v>146</v>
+        <v>8</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>147</v>
+        <v>9</v>
       </c>
       <c r="C12" s="12">
         <v>7</v>
@@ -1617,10 +1688,10 @@
     </row>
     <row r="13" spans="1:16" s="11" customFormat="1">
       <c r="A13" s="5" t="s">
-        <v>148</v>
+        <v>10</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>83</v>
+        <v>38</v>
       </c>
       <c r="C13" s="12">
         <v>7.1</v>
@@ -1644,10 +1715,10 @@
     </row>
     <row r="14" spans="1:16" s="10" customFormat="1">
       <c r="A14" s="5" t="s">
-        <v>84</v>
+        <v>39</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>85</v>
+        <v>40</v>
       </c>
       <c r="C14" s="12">
         <v>6</v>
@@ -1671,10 +1742,10 @@
     </row>
     <row r="15" spans="1:16" s="10" customFormat="1">
       <c r="A15" s="5" t="s">
-        <v>86</v>
+        <v>41</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>87</v>
+        <v>42</v>
       </c>
       <c r="C15" s="12">
         <v>6.1</v>
@@ -1698,10 +1769,10 @@
     </row>
     <row r="16" spans="1:16" s="5" customFormat="1">
       <c r="A16" s="6" t="s">
-        <v>86</v>
+        <v>41</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>88</v>
+        <v>43</v>
       </c>
       <c r="C16" s="7">
         <v>8</v>
@@ -1726,10 +1797,10 @@
     </row>
     <row r="17" spans="1:16" s="10" customFormat="1">
       <c r="A17" s="2" t="s">
-        <v>86</v>
+        <v>41</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>89</v>
+        <v>44</v>
       </c>
       <c r="C17" s="3">
         <v>8.75</v>
@@ -1754,10 +1825,10 @@
     </row>
     <row r="18" spans="1:16" s="10" customFormat="1">
       <c r="A18" s="2" t="s">
-        <v>90</v>
+        <v>45</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>91</v>
+        <v>46</v>
       </c>
       <c r="C18" s="3">
         <v>9.6999999999999993</v>
@@ -1782,10 +1853,10 @@
     </row>
     <row r="19" spans="1:16" s="10" customFormat="1">
       <c r="A19" s="6" t="s">
-        <v>92</v>
+        <v>47</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>143</v>
+        <v>5</v>
       </c>
       <c r="C19" s="7">
         <v>8.375</v>
@@ -1810,10 +1881,10 @@
     </row>
     <row r="20" spans="1:16" s="10" customFormat="1">
       <c r="A20" s="6" t="s">
-        <v>93</v>
+        <v>48</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>94</v>
+        <v>49</v>
       </c>
       <c r="C20" s="7">
         <v>7.9</v>
@@ -1838,10 +1909,10 @@
     </row>
     <row r="21" spans="1:16" s="10" customFormat="1">
       <c r="A21" s="5" t="s">
-        <v>95</v>
+        <v>50</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>96</v>
+        <v>51</v>
       </c>
       <c r="C21" s="12">
         <v>6.4</v>
@@ -1865,10 +1936,10 @@
     </row>
     <row r="22" spans="1:16" s="10" customFormat="1">
       <c r="A22" s="2" t="s">
-        <v>97</v>
+        <v>52</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>98</v>
+        <v>53</v>
       </c>
       <c r="C22" s="3">
         <v>8.1</v>
@@ -1893,10 +1964,10 @@
     </row>
     <row r="23" spans="1:16" s="2" customFormat="1">
       <c r="A23" s="2" t="s">
-        <v>99</v>
+        <v>54</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>100</v>
+        <v>55</v>
       </c>
       <c r="C23" s="3">
         <v>9.6999999999999993</v>
@@ -1920,10 +1991,10 @@
     </row>
     <row r="24" spans="1:16" s="10" customFormat="1">
       <c r="A24" s="6" t="s">
-        <v>101</v>
+        <v>56</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>102</v>
+        <v>57</v>
       </c>
       <c r="C24" s="7">
         <v>7.9</v>
@@ -1948,10 +2019,10 @@
     </row>
     <row r="25" spans="1:16" s="5" customFormat="1">
       <c r="A25" s="6" t="s">
-        <v>103</v>
+        <v>58</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>104</v>
+        <v>59</v>
       </c>
       <c r="C25" s="7">
         <v>8.625</v>
@@ -1976,10 +2047,10 @@
     </row>
     <row r="26" spans="1:16" s="2" customFormat="1">
       <c r="A26" s="2" t="s">
-        <v>105</v>
+        <v>60</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>106</v>
+        <v>61</v>
       </c>
       <c r="C26" s="3">
         <v>9.4</v>
@@ -2003,10 +2074,10 @@
     </row>
     <row r="27" spans="1:16" s="5" customFormat="1">
       <c r="A27" s="5" t="s">
-        <v>107</v>
+        <v>62</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>108</v>
+        <v>63</v>
       </c>
       <c r="C27" s="12">
         <v>7.1</v>
@@ -2031,10 +2102,10 @@
     </row>
     <row r="28" spans="1:16" s="5" customFormat="1">
       <c r="A28" s="6" t="s">
-        <v>109</v>
+        <v>64</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>110</v>
+        <v>65</v>
       </c>
       <c r="C28" s="6">
         <v>7.5</v>
@@ -2059,10 +2130,10 @@
     </row>
     <row r="29" spans="1:16" s="10" customFormat="1">
       <c r="A29" s="5" t="s">
-        <v>111</v>
+        <v>66</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>112</v>
+        <v>67</v>
       </c>
       <c r="C29" s="12">
         <v>6.75</v>
@@ -2086,10 +2157,10 @@
     </row>
     <row r="30" spans="1:16" s="10" customFormat="1">
       <c r="A30" s="5" t="s">
-        <v>113</v>
+        <v>68</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>114</v>
+        <v>69</v>
       </c>
       <c r="C30" s="12">
         <v>5.6</v>
@@ -2113,10 +2184,10 @@
     </row>
     <row r="31" spans="1:16" s="2" customFormat="1">
       <c r="A31" s="6" t="s">
-        <v>113</v>
+        <v>68</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>115</v>
+        <v>70</v>
       </c>
       <c r="C31" s="7">
         <v>7.5</v>
@@ -2139,10 +2210,10 @@
     </row>
     <row r="32" spans="1:16" s="2" customFormat="1">
       <c r="A32" s="5" t="s">
-        <v>48</v>
+        <v>141</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>49</v>
+        <v>142</v>
       </c>
       <c r="C32" s="12">
         <v>7.8</v>
@@ -2167,10 +2238,10 @@
     </row>
     <row r="33" spans="1:9" s="2" customFormat="1">
       <c r="A33" s="6" t="s">
-        <v>50</v>
+        <v>143</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>51</v>
+        <v>144</v>
       </c>
       <c r="C33" s="7">
         <v>7.2</v>
@@ -2193,10 +2264,10 @@
     </row>
     <row r="34" spans="1:9" s="2" customFormat="1">
       <c r="A34" s="2" t="s">
-        <v>52</v>
+        <v>145</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>53</v>
+        <v>146</v>
       </c>
       <c r="C34" s="3">
         <v>9.6</v>
@@ -2221,10 +2292,10 @@
     </row>
     <row r="35" spans="1:9" s="2" customFormat="1">
       <c r="A35" s="5" t="s">
-        <v>54</v>
+        <v>147</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>55</v>
+        <v>148</v>
       </c>
       <c r="C35" s="12">
         <v>6.875</v>
@@ -2248,10 +2319,10 @@
     </row>
     <row r="36" spans="1:9" s="10" customFormat="1">
       <c r="A36" s="6" t="s">
-        <v>56</v>
+        <v>149</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>57</v>
+        <v>150</v>
       </c>
       <c r="C36" s="7">
         <v>7.25</v>
@@ -2275,10 +2346,10 @@
     </row>
     <row r="37" spans="1:9" s="2" customFormat="1">
       <c r="A37" s="5" t="s">
-        <v>58</v>
+        <v>151</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>59</v>
+        <v>152</v>
       </c>
       <c r="C37" s="12">
         <v>6.1</v>
@@ -2304,10 +2375,10 @@
     </row>
     <row r="38" spans="1:9" s="2" customFormat="1">
       <c r="A38" s="5" t="s">
-        <v>60</v>
+        <v>153</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>61</v>
+        <v>154</v>
       </c>
       <c r="C38" s="12">
         <v>7.4</v>
@@ -2331,10 +2402,10 @@
     </row>
     <row r="39" spans="1:9" s="2" customFormat="1">
       <c r="A39" s="2" t="s">
-        <v>62</v>
+        <v>155</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>63</v>
+        <v>156</v>
       </c>
       <c r="C39" s="3">
         <v>8.4</v>
@@ -2357,10 +2428,10 @@
     </row>
     <row r="40" spans="1:9" s="2" customFormat="1">
       <c r="A40" s="6" t="s">
-        <v>64</v>
+        <v>157</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>65</v>
+        <v>158</v>
       </c>
       <c r="C40" s="7">
         <v>7.5</v>
@@ -2383,10 +2454,10 @@
     </row>
     <row r="41" spans="1:9" s="2" customFormat="1">
       <c r="A41" s="6" t="s">
-        <v>64</v>
+        <v>157</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>66</v>
+        <v>159</v>
       </c>
       <c r="C41" s="7">
         <v>8.6999999999999993</v>
@@ -2410,10 +2481,10 @@
     </row>
     <row r="42" spans="1:9" s="2" customFormat="1">
       <c r="A42" s="2" t="s">
-        <v>64</v>
+        <v>157</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>67</v>
+        <v>160</v>
       </c>
       <c r="C42" s="3">
         <v>8.8000000000000007</v>
@@ -2436,10 +2507,10 @@
     </row>
     <row r="43" spans="1:9" s="2" customFormat="1">
       <c r="A43" s="5" t="s">
-        <v>68</v>
+        <v>161</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>69</v>
+        <v>162</v>
       </c>
       <c r="C43" s="12">
         <v>7.8</v>
@@ -2464,10 +2535,10 @@
     </row>
     <row r="44" spans="1:9">
       <c r="A44" s="6" t="s">
-        <v>70</v>
+        <v>163</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>71</v>
+        <v>164</v>
       </c>
       <c r="C44" s="7">
         <v>8.1</v>
@@ -2491,10 +2562,10 @@
     </row>
     <row r="45" spans="1:9">
       <c r="A45" s="5" t="s">
-        <v>72</v>
+        <v>27</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>73</v>
+        <v>28</v>
       </c>
       <c r="C45" s="12">
         <v>6.25</v>
@@ -2518,10 +2589,10 @@
     </row>
     <row r="46" spans="1:9">
       <c r="A46" s="2" t="s">
-        <v>74</v>
+        <v>29</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>75</v>
+        <v>30</v>
       </c>
       <c r="C46" s="3">
         <v>8.8000000000000007</v>
@@ -2545,10 +2616,10 @@
     </row>
     <row r="47" spans="1:9">
       <c r="A47" s="6" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>77</v>
+        <v>32</v>
       </c>
       <c r="C47" s="7">
         <v>8.5</v>
@@ -2573,10 +2644,10 @@
     </row>
     <row r="48" spans="1:9">
       <c r="A48" s="5" t="s">
-        <v>78</v>
+        <v>33</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>79</v>
+        <v>34</v>
       </c>
       <c r="C48" s="12">
         <v>6.2</v>
@@ -2600,10 +2671,10 @@
     </row>
     <row r="49" spans="1:15">
       <c r="A49" s="6" t="s">
-        <v>80</v>
+        <v>35</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>81</v>
+        <v>36</v>
       </c>
       <c r="C49" s="7">
         <v>8.3000000000000007</v>
@@ -2627,10 +2698,10 @@
     </row>
     <row r="50" spans="1:15" s="2" customFormat="1">
       <c r="A50" s="6" t="s">
-        <v>82</v>
+        <v>37</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>13</v>
+        <v>106</v>
       </c>
       <c r="C50" s="7">
         <v>7.7</v>
@@ -2653,10 +2724,10 @@
     </row>
     <row r="51" spans="1:15" s="2" customFormat="1">
       <c r="A51" s="6" t="s">
-        <v>14</v>
+        <v>107</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>15</v>
+        <v>108</v>
       </c>
       <c r="C51" s="7">
         <v>8.625</v>
@@ -2679,10 +2750,10 @@
     </row>
     <row r="52" spans="1:15" s="2" customFormat="1">
       <c r="A52" s="2" t="s">
-        <v>16</v>
+        <v>109</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>17</v>
+        <v>110</v>
       </c>
       <c r="C52" s="3">
         <v>9.1999999999999993</v>
@@ -2705,10 +2776,10 @@
     </row>
     <row r="53" spans="1:15" s="2" customFormat="1">
       <c r="A53" s="6" t="s">
-        <v>18</v>
+        <v>111</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>19</v>
+        <v>112</v>
       </c>
       <c r="C53" s="7">
         <v>7.9</v>
@@ -2732,10 +2803,10 @@
     </row>
     <row r="54" spans="1:15" s="2" customFormat="1">
       <c r="A54" s="5" t="s">
-        <v>20</v>
+        <v>113</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>21</v>
+        <v>114</v>
       </c>
       <c r="C54" s="12">
         <v>7.5</v>
@@ -2758,10 +2829,10 @@
     </row>
     <row r="55" spans="1:15" s="2" customFormat="1">
       <c r="A55" s="6" t="s">
-        <v>22</v>
+        <v>115</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>23</v>
+        <v>116</v>
       </c>
       <c r="C55" s="7">
         <v>7.5</v>
@@ -2785,10 +2856,10 @@
     </row>
     <row r="56" spans="1:15" s="2" customFormat="1">
       <c r="A56" s="2" t="s">
-        <v>24</v>
+        <v>117</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>15</v>
+        <v>108</v>
       </c>
       <c r="C56" s="3">
         <v>10</v>
@@ -2813,10 +2884,10 @@
     </row>
     <row r="57" spans="1:15" s="2" customFormat="1">
       <c r="A57" s="6" t="s">
-        <v>25</v>
+        <v>118</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>26</v>
+        <v>119</v>
       </c>
       <c r="C57" s="7">
         <v>7.9</v>
@@ -2840,10 +2911,10 @@
     </row>
     <row r="58" spans="1:15" s="2" customFormat="1">
       <c r="A58" s="2" t="s">
-        <v>27</v>
+        <v>120</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>28</v>
+        <v>121</v>
       </c>
       <c r="C58" s="3">
         <v>9.5</v>
@@ -2866,10 +2937,10 @@
     </row>
     <row r="59" spans="1:15" s="2" customFormat="1">
       <c r="A59" s="6" t="s">
-        <v>29</v>
+        <v>122</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>30</v>
+        <v>123</v>
       </c>
       <c r="C59" s="7">
         <v>8.6</v>
@@ -2892,10 +2963,10 @@
     </row>
     <row r="60" spans="1:15" s="2" customFormat="1">
       <c r="A60" s="6" t="s">
-        <v>31</v>
+        <v>124</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>69</v>
+        <v>162</v>
       </c>
       <c r="C60" s="7">
         <v>8</v>
@@ -2919,10 +2990,10 @@
     </row>
     <row r="61" spans="1:15" s="2" customFormat="1">
       <c r="A61" s="6" t="s">
-        <v>32</v>
+        <v>125</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>33</v>
+        <v>126</v>
       </c>
       <c r="C61" s="7">
         <v>7.9</v>
@@ -2948,10 +3019,10 @@
     </row>
     <row r="62" spans="1:15" s="2" customFormat="1">
       <c r="A62" s="2" t="s">
-        <v>34</v>
+        <v>127</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>35</v>
+        <v>128</v>
       </c>
       <c r="C62" s="3">
         <v>8.6</v>
@@ -2974,10 +3045,10 @@
     </row>
     <row r="63" spans="1:15" s="2" customFormat="1">
       <c r="A63" s="5" t="s">
-        <v>36</v>
+        <v>129</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>37</v>
+        <v>130</v>
       </c>
       <c r="C63" s="12">
         <v>5.5</v>
@@ -3002,10 +3073,10 @@
     </row>
     <row r="64" spans="1:15" s="2" customFormat="1">
       <c r="A64" s="6" t="s">
-        <v>38</v>
+        <v>131</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>39</v>
+        <v>132</v>
       </c>
       <c r="C64" s="7">
         <v>8.25</v>
@@ -3028,10 +3099,10 @@
     </row>
     <row r="65" spans="1:15" s="2" customFormat="1">
       <c r="A65" s="2" t="s">
-        <v>40</v>
+        <v>133</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>41</v>
+        <v>134</v>
       </c>
       <c r="C65" s="3">
         <v>9.3000000000000007</v>
@@ -3057,10 +3128,10 @@
     </row>
     <row r="66" spans="1:15" s="2" customFormat="1">
       <c r="A66" s="5" t="s">
-        <v>42</v>
+        <v>135</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>43</v>
+        <v>136</v>
       </c>
       <c r="C66" s="12">
         <v>6.9</v>
@@ -3084,10 +3155,10 @@
     </row>
     <row r="67" spans="1:15" s="2" customFormat="1">
       <c r="A67" s="2" t="s">
-        <v>44</v>
+        <v>137</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>45</v>
+        <v>138</v>
       </c>
       <c r="C67" s="3">
         <v>9</v>
@@ -3110,10 +3181,10 @@
     </row>
     <row r="68" spans="1:15" s="2" customFormat="1">
       <c r="A68" s="2" t="s">
-        <v>46</v>
+        <v>139</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>47</v>
+        <v>140</v>
       </c>
       <c r="C68" s="3">
         <v>9.125</v>
@@ -3136,10 +3207,10 @@
     </row>
     <row r="69" spans="1:15" s="2" customFormat="1">
       <c r="A69" s="2" t="s">
-        <v>0</v>
+        <v>93</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>1</v>
+        <v>94</v>
       </c>
       <c r="C69" s="3">
         <v>8.5</v>
@@ -3162,10 +3233,10 @@
     </row>
     <row r="70" spans="1:15" s="2" customFormat="1">
       <c r="A70" s="5" t="s">
-        <v>2</v>
+        <v>95</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>3</v>
+        <v>96</v>
       </c>
       <c r="C70" s="12">
         <v>7.3</v>
@@ -3189,10 +3260,10 @@
     </row>
     <row r="71" spans="1:15" s="2" customFormat="1">
       <c r="A71" s="2" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>5</v>
+        <v>98</v>
       </c>
       <c r="C71" s="16">
         <v>9.25</v>
@@ -3204,21 +3275,21 @@
         <v>5.625</v>
       </c>
       <c r="F71" s="17" t="s">
-        <v>6</v>
+        <v>99</v>
       </c>
       <c r="G71" s="17" t="s">
-        <v>7</v>
+        <v>100</v>
       </c>
       <c r="H71" s="17" t="s">
-        <v>8</v>
+        <v>101</v>
       </c>
     </row>
     <row r="72" spans="1:15" s="2" customFormat="1">
       <c r="A72" s="2" t="s">
-        <v>9</v>
+        <v>102</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>10</v>
+        <v>103</v>
       </c>
       <c r="C72" s="3">
         <v>8.1999999999999993</v>
@@ -3241,10 +3312,10 @@
     </row>
     <row r="73" spans="1:15" s="2" customFormat="1">
       <c r="A73" s="2" t="s">
-        <v>11</v>
+        <v>104</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>12</v>
+        <v>105</v>
       </c>
       <c r="C73" s="3">
         <v>10</v>
@@ -3265,9 +3336,145 @@
         <v>0</v>
       </c>
     </row>
+    <row r="74" spans="1:15">
+      <c r="A74" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B74" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="C74" s="19">
+        <v>8.6</v>
+      </c>
+      <c r="D74" s="19">
+        <v>8.6</v>
+      </c>
+      <c r="E74" s="19">
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="75" spans="1:15">
+      <c r="A75" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B75" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C75" s="19">
+        <v>9</v>
+      </c>
+      <c r="D75" s="19">
+        <v>6</v>
+      </c>
+      <c r="E75" s="19">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="76" spans="1:15">
+      <c r="A76" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B76" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C76" s="19">
+        <v>7.8</v>
+      </c>
+      <c r="D76" s="19">
+        <v>6.6</v>
+      </c>
+      <c r="E76" s="19">
+        <v>8.3000000000000007</v>
+      </c>
+    </row>
+    <row r="77" spans="1:15">
+      <c r="A77" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B77" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C77" s="19">
+        <v>9.4</v>
+      </c>
+      <c r="D77" s="19">
+        <v>9.4</v>
+      </c>
+      <c r="E77" s="19">
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="78" spans="1:15">
+      <c r="A78" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B78" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C78" s="19">
+        <v>6.1</v>
+      </c>
+      <c r="D78" s="19">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="E78" s="19">
+        <v>8.4</v>
+      </c>
+    </row>
+    <row r="79" spans="1:15">
+      <c r="A79" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B79" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C79" s="19">
+        <v>6.5</v>
+      </c>
+      <c r="D79" s="19">
+        <v>6.5</v>
+      </c>
+      <c r="E79" s="19">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="80" spans="1:15">
+      <c r="A80" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B80" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C80" s="19">
+        <v>7.7</v>
+      </c>
+      <c r="D80" s="19">
+        <v>6.9</v>
+      </c>
+      <c r="E80" s="19">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
+      <c r="A81" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B81" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C81" s="19">
+        <v>4.5</v>
+      </c>
+      <c r="D81" s="19">
+        <v>3</v>
+      </c>
+      <c r="E81" s="19">
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
   </sheetData>
   <sheetCalcPr fullCalcOnLoad="1"/>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>

</xml_diff>